<commit_message>
added details, delete and edit view
</commit_message>
<xml_diff>
--- a/Coding.Lizards.Pokemon.Tools.Web/Strings/Texts.xlsx
+++ b/Coding.Lizards.Pokemon.Tools.Web/Strings/Texts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="160">
   <si>
     <t>Account_Login_Title</t>
   </si>
@@ -384,15 +384,9 @@
     <t>Pokemon_List_BaseAttack</t>
   </si>
   <si>
-    <t>Basis Attacke</t>
-  </si>
-  <si>
     <t>Pokemon_List_BaseSpecialAttack</t>
   </si>
   <si>
-    <t>Basis Spezialattacke</t>
-  </si>
-  <si>
     <t>Pokemon_List_BaseSpecialDefense</t>
   </si>
   <si>
@@ -436,6 +430,75 @@
   </si>
   <si>
     <t>Pokemon_List_Actions</t>
+  </si>
+  <si>
+    <t>Pokemon_Add_Title</t>
+  </si>
+  <si>
+    <t>Pokemon_Add_Submit</t>
+  </si>
+  <si>
+    <t>Pokemon_Add_Cancel</t>
+  </si>
+  <si>
+    <t>Pokemon_Add_BaseValues</t>
+  </si>
+  <si>
+    <t>Basiswerte</t>
+  </si>
+  <si>
+    <t>Basis Angriff</t>
+  </si>
+  <si>
+    <t>Basis Spezialangriff</t>
+  </si>
+  <si>
+    <t>Pokemon_Details_Title</t>
+  </si>
+  <si>
+    <t>Pokemon_Details_BaseValues</t>
+  </si>
+  <si>
+    <t>Enums_XpType_Fast</t>
+  </si>
+  <si>
+    <t>Schnell</t>
+  </si>
+  <si>
+    <t>Enums_XpType_MediumFast</t>
+  </si>
+  <si>
+    <t>Mittel-Schnell</t>
+  </si>
+  <si>
+    <t>Enums_XpType_MediumSlow</t>
+  </si>
+  <si>
+    <t>Mittel-Langsam</t>
+  </si>
+  <si>
+    <t>Enums_XpType_Slow</t>
+  </si>
+  <si>
+    <t>Langsam</t>
+  </si>
+  <si>
+    <t>Enums_XpType_Erratic</t>
+  </si>
+  <si>
+    <t>Erratic</t>
+  </si>
+  <si>
+    <t>Enums_XpType_Fluctuating</t>
+  </si>
+  <si>
+    <t>Fluctuating</t>
+  </si>
+  <si>
+    <t>Pokemon_List_ExperienceType</t>
+  </si>
+  <si>
+    <t>Erfahrungstyp</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,79 +1916,183 @@
         <v>120</v>
       </c>
       <c r="B70" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B71" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B72" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B73" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B74" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B75" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B76" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B78" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B79" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>137</v>
+      </c>
+      <c r="B80" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>138</v>
+      </c>
+      <c r="B81" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>144</v>
+      </c>
+      <c r="B84" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>145</v>
+      </c>
+      <c r="B85" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>146</v>
+      </c>
+      <c r="B86" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>150</v>
+      </c>
+      <c r="B88" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>156</v>
+      </c>
+      <c r="B91" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>158</v>
+      </c>
+      <c r="B92" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can calculate current status values
</commit_message>
<xml_diff>
--- a/Coding.Lizards.Pokemon.Tools.Web/Strings/Texts.xlsx
+++ b/Coding.Lizards.Pokemon.Tools.Web/Strings/Texts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="229">
   <si>
     <t>Account_Login_Title</t>
   </si>
@@ -700,6 +700,12 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>Pokemon_Details_ValuesOnLevel</t>
+  </si>
+  <si>
+    <t>Werte auf Level</t>
   </si>
 </sst>
 </file>
@@ -1549,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B139"/>
+  <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,6 +2679,14 @@
         <v>226</v>
       </c>
     </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>227</v>
+      </c>
+      <c r="B140" t="s">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:B35">
     <sortCondition ref="A35"/>

</xml_diff>

<commit_message>
added some startpage stuff
</commit_message>
<xml_diff>
--- a/Coding.Lizards.Pokemon.Tools.Web/Strings/Texts.xlsx
+++ b/Coding.Lizards.Pokemon.Tools.Web/Strings/Texts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="244">
   <si>
     <t>Account_Login_Title</t>
   </si>
@@ -706,6 +706,51 @@
   </si>
   <si>
     <t>Werte auf Level</t>
+  </si>
+  <si>
+    <t>Home_Index_Title</t>
+  </si>
+  <si>
+    <t>Startseite</t>
+  </si>
+  <si>
+    <t>Home_Index_Fight</t>
+  </si>
+  <si>
+    <t>Home_Index_XpCalc</t>
+  </si>
+  <si>
+    <t>Erfahrung</t>
+  </si>
+  <si>
+    <t>Home_Index_MyPokemon</t>
+  </si>
+  <si>
+    <t>Mein Pokémon</t>
+  </si>
+  <si>
+    <t>Home_Index_OpponentPokemon</t>
+  </si>
+  <si>
+    <t>Gegnerisches Pokémon</t>
+  </si>
+  <si>
+    <t>Home_Index_UsedAttack</t>
+  </si>
+  <si>
+    <t>Eingesetzte Attacke</t>
+  </si>
+  <si>
+    <t>Home_Index_Level</t>
+  </si>
+  <si>
+    <t>Home_Index_Pokemon</t>
+  </si>
+  <si>
+    <t>Home_Index_SearchPokemon</t>
+  </si>
+  <si>
+    <t>Pokémon suchen</t>
   </si>
 </sst>
 </file>
@@ -1555,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B140"/>
+  <dimension ref="A1:B149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A149" sqref="A149:B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,6 +2732,78 @@
         <v>228</v>
       </c>
     </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>229</v>
+      </c>
+      <c r="B141" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>231</v>
+      </c>
+      <c r="B142" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>232</v>
+      </c>
+      <c r="B143" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>234</v>
+      </c>
+      <c r="B144" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>236</v>
+      </c>
+      <c r="B145" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>238</v>
+      </c>
+      <c r="B146" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>240</v>
+      </c>
+      <c r="B147" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>241</v>
+      </c>
+      <c r="B148" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>242</v>
+      </c>
+      <c r="B149" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:B35">
     <sortCondition ref="A35"/>

</xml_diff>

<commit_message>
can calculate damage now
</commit_message>
<xml_diff>
--- a/Coding.Lizards.Pokemon.Tools.Web/Strings/Texts.xlsx
+++ b/Coding.Lizards.Pokemon.Tools.Web/Strings/Texts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="250">
   <si>
     <t>Account_Login_Title</t>
   </si>
@@ -751,6 +751,24 @@
   </si>
   <si>
     <t>Pokémon suchen</t>
+  </si>
+  <si>
+    <t>Home_Index_SearchAttack</t>
+  </si>
+  <si>
+    <t>Attacke suchen</t>
+  </si>
+  <si>
+    <t>Home_Index_MinDamage</t>
+  </si>
+  <si>
+    <t>Minimaler Schaden</t>
+  </si>
+  <si>
+    <t>Home_Index_MaxDamage</t>
+  </si>
+  <si>
+    <t>Maximaler Schaden</t>
   </si>
 </sst>
 </file>
@@ -1600,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B149"/>
+  <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149:B149"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A152" sqref="A151:B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,6 +2822,30 @@
         <v>243</v>
       </c>
     </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>244</v>
+      </c>
+      <c r="B150" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>246</v>
+      </c>
+      <c r="B151" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>248</v>
+      </c>
+      <c r="B152" t="s">
+        <v>249</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:B35">
     <sortCondition ref="A35"/>

</xml_diff>